<commit_message>
life exp 2021 and age distr
</commit_message>
<xml_diff>
--- a/data/file_life_expectancy_2021.xlsx
+++ b/data/file_life_expectancy_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aditharun/Documents/GitHub/cdc-wonder-mortality/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF4F7D5F-A0FF-5C48-8CDC-58DAF0BABF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3147F2-B036-1D46-9D16-CBA4F26CAC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8420" yWindow="1780" windowWidth="26820" windowHeight="16400" xr2:uid="{053C0B33-1532-2145-9329-E753D1F3378C}"/>
+    <workbookView xWindow="23260" yWindow="1780" windowWidth="11980" windowHeight="16900" xr2:uid="{053C0B33-1532-2145-9329-E753D1F3378C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{543D62A9-97A3-0542-95A2-8DAE9808A4F6}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>79.5</v>
+        <v>79.3</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>78.8</v>
+        <v>78.7</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -500,7 +500,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>69.900000000000006</v>
+        <v>69.8</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -668,7 +668,7 @@
         <v>70</v>
       </c>
       <c r="C17">
-        <v>15.9</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -682,7 +682,7 @@
         <v>75</v>
       </c>
       <c r="C18">
-        <v>12.4</v>
+        <v>12.5</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -696,7 +696,7 @@
         <v>80</v>
       </c>
       <c r="C19">
-        <v>9.3000000000000007</v>
+        <v>9.4</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -710,7 +710,7 @@
         <v>85</v>
       </c>
       <c r="C20">
-        <v>6.6</v>
+        <v>6.7</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -724,7 +724,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>74</v>
+        <v>73.5</v>
       </c>
       <c r="D21" t="s">
         <v>5</v>
@@ -738,7 +738,7 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>73.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>5</v>
@@ -752,7 +752,7 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>69.400000000000006</v>
+        <v>69.099999999999994</v>
       </c>
       <c r="D23" t="s">
         <v>5</v>
@@ -766,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>64.5</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="D24" t="s">
         <v>5</v>
@@ -780,7 +780,7 @@
         <v>15</v>
       </c>
       <c r="C25">
-        <v>59.5</v>
+        <v>59.2</v>
       </c>
       <c r="D25" t="s">
         <v>5</v>
@@ -794,7 +794,7 @@
         <v>20</v>
       </c>
       <c r="C26">
-        <v>54.7</v>
+        <v>54.4</v>
       </c>
       <c r="D26" t="s">
         <v>5</v>
@@ -808,7 +808,7 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>50.1</v>
+        <v>49.8</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
@@ -822,7 +822,7 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>45.6</v>
+        <v>45.4</v>
       </c>
       <c r="D28" t="s">
         <v>5</v>
@@ -836,7 +836,7 @@
         <v>35</v>
       </c>
       <c r="C29">
-        <v>41.2</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
         <v>5</v>
@@ -850,7 +850,7 @@
         <v>40</v>
       </c>
       <c r="C30">
-        <v>36.799999999999997</v>
+        <v>36.6</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
@@ -864,7 +864,7 @@
         <v>45</v>
       </c>
       <c r="C31">
-        <v>32.5</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="D31" t="s">
         <v>5</v>
@@ -878,7 +878,7 @@
         <v>50</v>
       </c>
       <c r="C32">
-        <v>28.3</v>
+        <v>28.2</v>
       </c>
       <c r="D32" t="s">
         <v>5</v>
@@ -892,7 +892,7 @@
         <v>55</v>
       </c>
       <c r="C33">
-        <v>24.3</v>
+        <v>24.2</v>
       </c>
       <c r="D33" t="s">
         <v>5</v>
@@ -962,7 +962,7 @@
         <v>80</v>
       </c>
       <c r="C38">
-        <v>7.8</v>
+        <v>7.9</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>

</xml_diff>